<commit_message>
decreased timing of pic to 2 seconds, decreased total events to 45
</commit_message>
<xml_diff>
--- a/conditions.xlsx
+++ b/conditions.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="2240" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="81">
   <si>
     <t>images</t>
   </si>
@@ -638,13 +638,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -815,14 +819,14 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
         <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>7</v>
@@ -830,153 +834,153 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>7</v>
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D16" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D18" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D20" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D21" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D22" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D23" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D24" t="s">
         <v>15</v>
@@ -984,195 +988,195 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="D25" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" t="s">
-        <v>11</v>
+      <c r="A26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>7</v>
+      <c r="A27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="D28" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C30" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="D30" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="B31" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="C31" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="D31" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="C32" t="s">
-        <v>18</v>
+        <v>75</v>
       </c>
       <c r="D32" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B33" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C33" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D33" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="B34" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="C34" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="D34" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="C35" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="D35" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B36" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C36" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D36" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C37" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D37" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="B38" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="C38" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="D38" t="s">
         <v>15</v>
@@ -1180,13 +1184,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" t="s">
         <v>77</v>
-      </c>
-      <c r="C39" t="s">
-        <v>61</v>
       </c>
       <c r="D39" t="s">
         <v>11</v>
@@ -1194,82 +1198,82 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="B40" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="C40" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D40" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="B41" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="C41" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="D41" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="B42" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>77</v>
-      </c>
-      <c r="D42" t="s">
-        <v>11</v>
+        <v>80</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="B43" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="C43" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="D43" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="C44" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" t="s">
+      <c r="A45" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B45" t="s">
-        <v>40</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="C45" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -1278,57 +1282,15 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="B46" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="C46" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="D46" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" t="s">
-        <v>69</v>
-      </c>
-      <c r="B47" t="s">
-        <v>22</v>
-      </c>
-      <c r="C47" t="s">
-        <v>68</v>
-      </c>
-      <c r="D47" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" t="s">
-        <v>74</v>
-      </c>
-      <c r="B49" t="s">
-        <v>78</v>
-      </c>
-      <c r="C49" t="s">
-        <v>75</v>
-      </c>
-      <c r="D49" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>